<commit_message>
Thêm giá trị và tổng tiền Voucher
</commit_message>
<xml_diff>
--- a/Media/Template/Template-rpt_Voucher_Sync.xlsx
+++ b/Media/Template/Template-rpt_Voucher_Sync.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DuyTu_E\SourceCode\VOUCHER_CENTER\Media\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325EEB49-A7BE-46FC-9669-F9692DF8917E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C809DB5C-A89A-4002-B75B-C3D4E8A61B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-6150" windowWidth="29040" windowHeight="15840" xr2:uid="{F2271192-5DF1-4A71-AFAF-54365E7BC0E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F2271192-5DF1-4A71-AFAF-54365E7BC0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="10" r:id="rId1"/>
@@ -44,55 +44,55 @@
     <t>Id</t>
   </si>
   <si>
-    <t>User_Name</t>
-  </si>
-  <si>
-    <t>TRANS_NUM</t>
-  </si>
-  <si>
-    <t>Voucher_Serial</t>
-  </si>
-  <si>
-    <t>Voucher_Code</t>
-  </si>
-  <si>
-    <t>Created_Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Computer_name</t>
-  </si>
-  <si>
-    <t>Player_Name</t>
-  </si>
-  <si>
-    <t>Locations_Group</t>
-  </si>
-  <si>
-    <t>Location_GroupName</t>
-  </si>
-  <si>
-    <t>Locations_Detail</t>
-  </si>
-  <si>
-    <t>Location_DetailName</t>
-  </si>
-  <si>
-    <t>Cancelled_Date</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Last_update</t>
-  </si>
-  <si>
     <t>Sync</t>
   </si>
   <si>
     <t>BÁO CÁO E VOUCHER ĐÃ CẬP NHẬT</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập</t>
+  </si>
+  <si>
+    <t>Mã giao dịch</t>
+  </si>
+  <si>
+    <t>Số Voucher</t>
+  </si>
+  <si>
+    <t>Ngày tạo</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Tên trạm sử dụng</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>Mã Cty</t>
+  </si>
+  <si>
+    <t>Tên Cty</t>
+  </si>
+  <si>
+    <t>Mã CH</t>
+  </si>
+  <si>
+    <t>Tên Cửa hàng</t>
+  </si>
+  <si>
+    <t>Huỷ</t>
+  </si>
+  <si>
+    <t>Diễn giải</t>
+  </si>
+  <si>
+    <t>Cập nhật lần cuối</t>
+  </si>
+  <si>
+    <t>Mệnh giá</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,12 +220,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -262,6 +256,12 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,17 +277,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -607,27 +601,27 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.5703125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="41.5703125" style="5" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.42578125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="27.85546875" style="14" customWidth="1"/>
+    <col min="15" max="15" width="41.42578125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" style="12" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -637,19 +631,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="21"/>
-      <c r="C1" s="25">
+      <c r="C1" s="22">
         <f>M6</f>
         <v>0</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="3"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="3" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -680,85 +670,90 @@
       <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="12"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:M5" xr:uid="{7A6CB1E3-818C-4958-B0C5-CDE5AA3EB50C}"/>
@@ -766,7 +761,7 @@
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>